<commit_message>
Merged PR 9456: BP-789 Campaign Export to Excel - Calculate Units
BP-789 implementation and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_30SecEquivalizedAndNot.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_30SecEquivalizedAndNot.xlsx
@@ -250,7 +250,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 07/03/20</t>
+    <t>Created 08/05/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -605,318 +605,318 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="106">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="4" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="4" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="6" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="7" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="7" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="13" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="13" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="4" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="4" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="14" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="14" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="13" applyBorder="1" xfId="0">
+    <xf numFmtId="14" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="8" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="8" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="13" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="13" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="13" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="9" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="6" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="13" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="6" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="13" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
     </xf>
-    <xf numFmtId="167" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="167" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="167" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="167" applyNumberFormat="1" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="2"/>
     </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="167" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="168" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="5" applyFill="1" borderId="9" applyBorder="1" xfId="0">
+    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="168" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="5" applyFill="1" borderId="9" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="1" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="15" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="11" applyBorder="1" xfId="0">
+    <xf numFmtId="1" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="15" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="11" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="10" applyBorder="1" xfId="0">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="14" applyBorder="1" xfId="0">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="9" applyFont="1" fillId="6" applyFill="1" borderId="14" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="12" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="12" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1514,7 +1514,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 07/03/20</v>
+        <v>Created 08/05/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -1679,46 +1679,46 @@
         <v>23</v>
       </c>
       <c r="C10" s="67">
-        <v>0</v>
+        <v>0.1568</v>
       </c>
       <c r="D10" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="E10" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="F10" s="59">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="G10" s="67">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="H10" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="I10" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="J10" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="K10" s="59">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="L10" s="67">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="M10" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="N10" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="O10" s="59">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="P10" s="59">
-        <v>0</v>
+        <v>1.9999999999999996</v>
       </c>
     </row>
     <row r="11" ht="24" customHeight="1">
@@ -2003,46 +2003,46 @@
         <v>23</v>
       </c>
       <c r="C19" s="67">
-        <v>0</v>
+        <v>0.1568</v>
       </c>
       <c r="D19" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="E19" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="F19" s="59">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="G19" s="67">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="H19" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="I19" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="J19" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="K19" s="59">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="L19" s="67">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="M19" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="N19" s="37">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="O19" s="59">
-        <v>0</v>
+        <v>0.1536</v>
       </c>
       <c r="P19" s="59">
-        <v>0</v>
+        <v>1.9999999999999996</v>
       </c>
     </row>
     <row r="20" ht="24" customHeight="1">
@@ -2337,37 +2337,37 @@
         <v>0</v>
       </c>
       <c r="D28" s="37">
-        <v>0</v>
+        <v>0.184</v>
       </c>
       <c r="E28" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="F28" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="G28" s="59">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="H28" s="67">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="I28" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="J28" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="K28" s="59">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="L28" s="67">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="M28" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="N28" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="O28" s="37">
         <v>0</v>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="59">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" ht="24" customHeight="1">
@@ -2681,37 +2681,37 @@
         <v>0</v>
       </c>
       <c r="D37" s="37">
-        <v>0</v>
+        <v>0.184</v>
       </c>
       <c r="E37" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="F37" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="G37" s="59">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="H37" s="67">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="I37" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="J37" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="K37" s="59">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="L37" s="67">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="M37" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="N37" s="37">
-        <v>0</v>
+        <v>0.1816</v>
       </c>
       <c r="O37" s="37">
         <v>0</v>
@@ -2720,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="59">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" ht="24" customHeight="1">
@@ -3272,13 +3272,13 @@
         <f>SUM(J9:J10)</f>
         <v>27669</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="47" t="e">
         <f>E11/J11</f>
-        <v>3.6914958979363188</v>
-      </c>
-      <c r="L11" s="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L11" s="43" t="e">
         <f>E11/H11</f>
-        <v>4426.1035816256463</v>
+        <v>#VALUE!</v>
       </c>
       <c r="M11" s="31"/>
       <c r="N11" s="45" t="s">
@@ -3298,13 +3298,13 @@
         <f>SUM(R9:R10)</f>
         <v>8189.91</v>
       </c>
-      <c r="S11" s="47">
+      <c r="S11" s="47" t="e">
         <f>E11/R11</f>
-        <v>12.471443520136363</v>
-      </c>
-      <c r="T11" s="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T11" s="43" t="e">
         <f>E11/P11</f>
-        <v>12482.667819304488</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" ht="24" customHeight="1">
@@ -3529,13 +3529,13 @@
         <f>SUM(J15:J16)</f>
         <v>24004</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="47" t="e">
         <f>E17/J17</f>
-        <v>4.78253624395934</v>
-      </c>
-      <c r="L17" s="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L17" s="43" t="e">
         <f>E17/H17</f>
-        <v>5734.2609565072489</v>
+        <v>#VALUE!</v>
       </c>
       <c r="M17" s="31"/>
       <c r="N17" s="45" t="s">
@@ -3555,13 +3555,13 @@
         <f>SUM(R15:R16)</f>
         <v>7099.380000000001</v>
       </c>
-      <c r="S17" s="47">
+      <c r="S17" s="47" t="e">
         <f>E17/R17</f>
-        <v>16.170426149889142</v>
-      </c>
-      <c r="T17" s="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T17" s="43" t="e">
         <f>E17/P17</f>
-        <v>16184.979533424046</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" ht="24" customHeight="1">
@@ -5546,7 +5546,7 @@
   </sheetPr>
   <dimension ref="A2:T30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0" tabSelected="1">
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0" tabSelected="0">
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
@@ -5754,43 +5754,43 @@
         <v>83</v>
       </c>
       <c r="E9" s="83">
-        <v>0</v>
+        <v>1.9999999999999996</v>
       </c>
       <c r="F9" s="84">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G9" s="85">
         <v>12000</v>
       </c>
       <c r="H9" s="86">
-        <v>0</v>
+        <v>3.2000001024000033</v>
       </c>
       <c r="I9" s="87">
-        <v>6.3999999999999986</v>
+        <v>6.4000002048000049</v>
       </c>
       <c r="J9" s="83">
-        <v>0</v>
+        <v>3852.080123266564</v>
       </c>
       <c r="K9" s="83">
-        <v>7704.159999999998</v>
+        <v>7704.1602465331262</v>
       </c>
       <c r="L9" s="88">
-        <v>1.5576000498432017</v>
+        <v>1.5575999999999997</v>
       </c>
       <c r="M9" s="85">
-        <v>1875</v>
+        <v>1874.999940000002</v>
       </c>
       <c r="N9" s="89">
-        <v>0.64900002076800078</v>
+        <v>0.64900000000000013</v>
       </c>
       <c r="O9" s="86">
-        <v>0</v>
+        <v>1.95</v>
       </c>
       <c r="P9" s="87">
         <v>3.899999999999999</v>
       </c>
       <c r="Q9" s="83">
-        <v>0</v>
+        <v>2500.0000000000005</v>
       </c>
       <c r="R9" s="83">
         <v>5000</v>
@@ -5809,7 +5809,7 @@
         <v>84</v>
       </c>
       <c r="E10" s="51">
-        <v>0</v>
+        <v>1.9999999999999996</v>
       </c>
       <c r="F10" s="42" t="s">
         <v>38</v>
@@ -5821,19 +5821,19 @@
         <v>38</v>
       </c>
       <c r="I10" s="79">
-        <v>6.3999999999999986</v>
+        <v>6.4000002048000049</v>
       </c>
       <c r="J10" s="51" t="s">
         <v>38</v>
       </c>
       <c r="K10" s="51">
-        <v>7704.159999999998</v>
+        <v>7704.1602465331262</v>
       </c>
       <c r="L10" s="47">
-        <v>1.5576000498432017</v>
+        <v>1.5575999999999997</v>
       </c>
       <c r="M10" s="43">
-        <v>1875</v>
+        <v>1874.999940000002</v>
       </c>
       <c r="N10" s="45" t="s">
         <v>38</v>
@@ -5955,43 +5955,43 @@
         <v>83</v>
       </c>
       <c r="E14" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="84">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G14" s="85">
         <v>12000</v>
       </c>
       <c r="H14" s="86">
-        <v>0</v>
+        <v>3.2000001024000038</v>
       </c>
       <c r="I14" s="87">
-        <v>6.4000000000000021</v>
+        <v>6.4000002048000075</v>
       </c>
       <c r="J14" s="83">
-        <v>0</v>
+        <v>3852.0801232665635</v>
       </c>
       <c r="K14" s="83">
-        <v>7704.1600000000008</v>
+        <v>7704.1602465331271</v>
       </c>
       <c r="L14" s="88">
-        <v>1.5576000498432017</v>
+        <v>1.5575999999999997</v>
       </c>
       <c r="M14" s="85">
-        <v>1875</v>
+        <v>1874.9999399999992</v>
       </c>
       <c r="N14" s="89">
-        <v>0.64900002076800056</v>
+        <v>0.649</v>
       </c>
       <c r="O14" s="86">
-        <v>0</v>
+        <v>1.6499999999999997</v>
       </c>
       <c r="P14" s="87">
         <v>3.2999999999999994</v>
       </c>
       <c r="Q14" s="83">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="R14" s="83">
         <v>5000</v>
@@ -6010,7 +6010,7 @@
         <v>84</v>
       </c>
       <c r="E15" s="51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="42" t="s">
         <v>38</v>
@@ -6022,19 +6022,19 @@
         <v>38</v>
       </c>
       <c r="I15" s="79">
-        <v>6.4000000000000021</v>
+        <v>6.4000002048000075</v>
       </c>
       <c r="J15" s="51" t="s">
         <v>38</v>
       </c>
       <c r="K15" s="51">
-        <v>7704.1600000000008</v>
+        <v>7704.1602465331271</v>
       </c>
       <c r="L15" s="47">
-        <v>1.5576000498432017</v>
+        <v>1.5575999999999997</v>
       </c>
       <c r="M15" s="43">
-        <v>1875</v>
+        <v>1874.9999399999992</v>
       </c>
       <c r="N15" s="45" t="s">
         <v>38</v>
@@ -6156,43 +6156,43 @@
         <v>83</v>
       </c>
       <c r="E19" s="83">
-        <v>0</v>
+        <v>3.9999999999999996</v>
       </c>
       <c r="F19" s="84">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G19" s="85">
         <v>24000</v>
       </c>
       <c r="H19" s="86">
-        <v>0</v>
+        <v>6.4000002048000066</v>
       </c>
       <c r="I19" s="87">
-        <v>12.8</v>
+        <v>12.800000409600013</v>
       </c>
       <c r="J19" s="83">
-        <v>0</v>
+        <v>7704.1602465331271</v>
       </c>
       <c r="K19" s="83">
-        <v>15408.32</v>
+        <v>15408.320493066254</v>
       </c>
       <c r="L19" s="88">
-        <v>1.5576000498432017</v>
+        <v>1.5575999999999954</v>
       </c>
       <c r="M19" s="85">
-        <v>1875</v>
+        <v>1874.999940000002</v>
       </c>
       <c r="N19" s="89">
-        <v>0.64900002076800067</v>
+        <v>0.649</v>
       </c>
       <c r="O19" s="86">
-        <v>0</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="P19" s="87">
         <v>7.1999999999999984</v>
       </c>
       <c r="Q19" s="83">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="R19" s="83">
         <v>10000</v>
@@ -6211,7 +6211,7 @@
         <v>84</v>
       </c>
       <c r="E20" s="51">
-        <v>0</v>
+        <v>3.9999999999999996</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>38</v>
@@ -6223,19 +6223,19 @@
         <v>38</v>
       </c>
       <c r="I20" s="79">
-        <v>12.8</v>
+        <v>12.800000409600013</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>38</v>
       </c>
       <c r="K20" s="51">
-        <v>15408.32</v>
+        <v>15408.320493066254</v>
       </c>
       <c r="L20" s="47">
-        <v>1.5576000498432017</v>
+        <v>1.5575999999999954</v>
       </c>
       <c r="M20" s="43">
-        <v>1875</v>
+        <v>1874.999940000002</v>
       </c>
       <c r="N20" s="45" t="s">
         <v>38</v>

</xml_diff>